<commit_message>
Selenium automation on instagram using CacheLookUp annotation,data dr…
</commit_message>
<xml_diff>
--- a/src/main/resources/LoginDetailsOfInstagram.xlsx
+++ b/src/main/resources/LoginDetailsOfInstagram.xlsx
@@ -24,25 +24,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>surabhi12345</t>
+    <t>Theend@1</t>
   </si>
   <si>
-    <t>Surabhi@123</t>
-  </si>
-  <si>
-    <t>amruta12</t>
-  </si>
-  <si>
-    <t>Amruta@321</t>
+    <t>testingblz123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,12 +45,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,16 +68,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -367,36 +359,29 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>